<commit_message>
This resolves #41, resolves#42, resolves #43, resolves #44, resolves #29, resolves #30, resolves #32, resolves #33, resolves #34, resolves #35, resolves #36, resolves #37, resolves #38, resolves #39, resolves #27
</commit_message>
<xml_diff>
--- a/Test Cases/Negative Test Cases/Contacts Test Suite.xlsx
+++ b/Test Cases/Negative Test Cases/Contacts Test Suite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>Test Case № 1</t>
   </si>
@@ -49,9 +49,6 @@
     <t>No new messages received</t>
   </si>
   <si>
-    <t>5. Check if there is received Email with the message from №3</t>
-  </si>
-  <si>
     <t>Send email to the Web Admins without filling up message field</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Error "Please enter Message" appears</t>
   </si>
   <si>
-    <t>5. Check if there is received Email from the Email from step № 2</t>
-  </si>
-  <si>
     <t>Test Case № 2</t>
   </si>
   <si>
@@ -92,13 +86,22 @@
   </si>
   <si>
     <t>Error "Please enter valid Email address" appears</t>
+  </si>
+  <si>
+    <t>5. Check if there is received Admin message with the message from №3</t>
+  </si>
+  <si>
+    <t>5. Check if there is received Admin message from the Email from step № 2</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,13 +109,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,8 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,8 +469,11 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -498,7 +519,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -509,10 +530,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,7 +555,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -539,7 +563,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -553,12 +577,12 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -569,10 +593,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -591,7 +618,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -599,7 +626,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -613,12 +640,12 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -629,10 +656,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -651,7 +681,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -673,12 +703,12 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -689,5 +719,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This resolves #42, resolves #28, resolves #26, resolves #22
</commit_message>
<xml_diff>
--- a/Test Cases/Negative Test Cases/Contacts Test Suite.xlsx
+++ b/Test Cases/Negative Test Cases/Contacts Test Suite.xlsx
@@ -145,8 +145,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,15 +466,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -529,15 +530,16 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -592,15 +594,16 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -655,15 +658,16 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">

</xml_diff>